<commit_message>
TP#15226 Fixed the rest of the tests
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/US Exp Intl.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/US Exp Intl.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4290" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4288" uniqueCount="477">
   <si>
     <t>SaveLabel</t>
   </si>
@@ -1332,9 +1332,6 @@
     <t>IERC1</t>
   </si>
   <si>
-    <t>RETURNS_CLEARANCE</t>
-  </si>
-  <si>
     <t>OTHER</t>
   </si>
   <si>
@@ -1462,9 +1459,6 @@
   </si>
   <si>
     <t>THIRD PARTY CONSIGNEE</t>
-  </si>
-  <si>
-    <t>TRUE</t>
   </si>
 </sst>
 </file>
@@ -1932,7 +1926,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2174,9 +2168,6 @@
     <xf numFmtId="0" fontId="16" fillId="7" borderId="10" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -2515,10 +2506,10 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:ER65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="DF1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z1" sqref="Z1"/>
-      <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
+      <selection pane="bottomLeft" activeCell="DJ64" sqref="DJ64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3545,7 +3536,7 @@
       <c r="A3" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="99" t="s">
         <v>143</v>
       </c>
       <c r="C3" s="32"/>
@@ -3853,10 +3844,10 @@
       <c r="A4" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B4" s="101"/>
+      <c r="B4" s="100"/>
       <c r="C4" s="41"/>
       <c r="D4" s="32" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E4" s="33" t="s">
         <v>145</v>
@@ -4165,7 +4156,7 @@
       <c r="A5" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B5" s="101"/>
+      <c r="B5" s="100"/>
       <c r="C5" s="41"/>
       <c r="D5" s="32" t="s">
         <v>185</v>
@@ -4473,7 +4464,7 @@
       <c r="A6" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B6" s="101"/>
+      <c r="B6" s="100"/>
       <c r="C6" s="41"/>
       <c r="D6" s="32" t="s">
         <v>194</v>
@@ -4785,10 +4776,10 @@
       <c r="A7" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B7" s="101"/>
+      <c r="B7" s="100"/>
       <c r="C7" s="41"/>
       <c r="D7" s="32" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E7" s="33" t="s">
         <v>145</v>
@@ -5089,7 +5080,7 @@
         <v>1</v>
       </c>
       <c r="EA7" s="33" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="EB7" s="33" t="s">
         <v>212</v>
@@ -5145,10 +5136,10 @@
       <c r="A8" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B8" s="101"/>
+      <c r="B8" s="100"/>
       <c r="C8" s="41"/>
       <c r="D8" s="32" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E8" s="33" t="s">
         <v>145</v>
@@ -5459,10 +5450,10 @@
       <c r="A9" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B9" s="101"/>
+      <c r="B9" s="100"/>
       <c r="C9" s="41"/>
       <c r="D9" s="32" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E9" s="33" t="s">
         <v>145</v>
@@ -5775,10 +5766,10 @@
       <c r="A10" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B10" s="101"/>
+      <c r="B10" s="100"/>
       <c r="C10" s="41"/>
       <c r="D10" s="32" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E10" s="33" t="s">
         <v>145</v>
@@ -6071,7 +6062,7 @@
         <v>1</v>
       </c>
       <c r="EA10" s="33" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="EB10" s="33" t="s">
         <v>212</v>
@@ -6127,7 +6118,7 @@
       <c r="A11" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B11" s="101"/>
+      <c r="B11" s="100"/>
       <c r="C11" s="41"/>
       <c r="D11" s="32" t="s">
         <v>238</v>
@@ -6435,7 +6426,7 @@
       <c r="A12" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B12" s="101"/>
+      <c r="B12" s="100"/>
       <c r="C12" s="41"/>
       <c r="D12" s="32" t="s">
         <v>238</v>
@@ -6743,10 +6734,10 @@
       <c r="A13" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B13" s="101"/>
+      <c r="B13" s="100"/>
       <c r="C13" s="41"/>
       <c r="D13" s="32" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E13" s="33" t="s">
         <v>145</v>
@@ -7053,10 +7044,10 @@
       <c r="A14" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B14" s="101"/>
+      <c r="B14" s="100"/>
       <c r="C14" s="41"/>
       <c r="D14" s="32" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E14" s="33" t="s">
         <v>145</v>
@@ -7341,7 +7332,7 @@
         <v>1</v>
       </c>
       <c r="EA14" s="33" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="EB14" s="33" t="s">
         <v>212</v>
@@ -7397,10 +7388,10 @@
       <c r="A15" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B15" s="101"/>
+      <c r="B15" s="100"/>
       <c r="C15" s="41"/>
       <c r="D15" s="32" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E15" s="33" t="s">
         <v>145</v>
@@ -7719,10 +7710,10 @@
       <c r="A16" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B16" s="101"/>
+      <c r="B16" s="100"/>
       <c r="C16" s="41"/>
       <c r="D16" s="32" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E16" s="33" t="s">
         <v>145</v>
@@ -8027,7 +8018,7 @@
       <c r="A17" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B17" s="101"/>
+      <c r="B17" s="100"/>
       <c r="C17" s="41"/>
       <c r="D17" s="32" t="s">
         <v>371</v>
@@ -8333,7 +8324,7 @@
       <c r="A18" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B18" s="101"/>
+      <c r="B18" s="100"/>
       <c r="C18" s="41"/>
       <c r="D18" s="32" t="s">
         <v>296</v>
@@ -8639,10 +8630,10 @@
       <c r="A19" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="100"/>
       <c r="C19" s="41"/>
       <c r="D19" s="32" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E19" s="33" t="s">
         <v>145</v>
@@ -8949,10 +8940,10 @@
       <c r="A20" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B20" s="101"/>
+      <c r="B20" s="100"/>
       <c r="C20" s="41"/>
       <c r="D20" s="32" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E20" s="33" t="s">
         <v>145</v>
@@ -9267,7 +9258,7 @@
       <c r="A21" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B21" s="101"/>
+      <c r="B21" s="100"/>
       <c r="C21" s="41"/>
       <c r="D21" s="32" t="s">
         <v>276</v>
@@ -9575,10 +9566,10 @@
       <c r="A22" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B22" s="101"/>
+      <c r="B22" s="100"/>
       <c r="C22" s="41"/>
       <c r="D22" s="32" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E22" s="33" t="s">
         <v>145</v>
@@ -9885,10 +9876,10 @@
       <c r="A23" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B23" s="101"/>
+      <c r="B23" s="100"/>
       <c r="C23" s="41"/>
       <c r="D23" s="32" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E23" s="33" t="s">
         <v>145</v>
@@ -10010,7 +10001,7 @@
         <v>281</v>
       </c>
       <c r="AX23" s="35" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="AY23" s="37">
         <v>110001</v>
@@ -10207,10 +10198,10 @@
       <c r="A24" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B24" s="101"/>
+      <c r="B24" s="100"/>
       <c r="C24" s="41"/>
       <c r="D24" s="32" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E24" s="33" t="s">
         <v>145</v>
@@ -10521,10 +10512,10 @@
       <c r="A25" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B25" s="101"/>
+      <c r="B25" s="100"/>
       <c r="C25" s="41"/>
       <c r="D25" s="32" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E25" s="33" t="s">
         <v>145</v>
@@ -10813,7 +10804,7 @@
         <v>1</v>
       </c>
       <c r="EA25" s="33" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="EB25" s="33" t="s">
         <v>212</v>
@@ -10869,7 +10860,7 @@
       <c r="A26" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B26" s="101"/>
+      <c r="B26" s="100"/>
       <c r="C26" s="41"/>
       <c r="D26" s="32" t="s">
         <v>397</v>
@@ -11183,7 +11174,7 @@
       <c r="A27" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B27" s="101"/>
+      <c r="B27" s="100"/>
       <c r="C27" s="41"/>
       <c r="D27" s="32" t="s">
         <v>285</v>
@@ -11525,7 +11516,7 @@
       <c r="A28" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B28" s="101"/>
+      <c r="B28" s="100"/>
       <c r="C28" s="41"/>
       <c r="D28" s="32" t="s">
         <v>291</v>
@@ -11841,7 +11832,7 @@
       <c r="A29" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B29" s="101"/>
+      <c r="B29" s="100"/>
       <c r="C29" s="41"/>
       <c r="D29" s="32" t="s">
         <v>238</v>
@@ -12149,7 +12140,7 @@
       <c r="A30" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B30" s="101"/>
+      <c r="B30" s="100"/>
       <c r="C30" s="44"/>
       <c r="D30" s="32" t="s">
         <v>296</v>
@@ -12453,7 +12444,7 @@
       <c r="A31" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B31" s="101"/>
+      <c r="B31" s="100"/>
       <c r="C31" s="44"/>
       <c r="D31" s="32" t="s">
         <v>312</v>
@@ -12747,10 +12738,10 @@
       <c r="A32" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B32" s="101"/>
+      <c r="B32" s="100"/>
       <c r="C32" s="44"/>
       <c r="D32" s="32" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E32" s="33" t="s">
         <v>145</v>
@@ -13047,7 +13038,7 @@
         <v>1</v>
       </c>
       <c r="EA32" s="33" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="EB32" s="33" t="s">
         <v>212</v>
@@ -13103,7 +13094,7 @@
       <c r="A33" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B33" s="101"/>
+      <c r="B33" s="100"/>
       <c r="C33" s="41"/>
       <c r="D33" s="32" t="s">
         <v>144</v>
@@ -13413,10 +13404,10 @@
       <c r="A34" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B34" s="101"/>
+      <c r="B34" s="100"/>
       <c r="C34" s="44"/>
       <c r="D34" s="32" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E34" s="33" t="s">
         <v>145</v>
@@ -13737,10 +13728,10 @@
       <c r="A35" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B35" s="101"/>
+      <c r="B35" s="100"/>
       <c r="C35" s="44"/>
       <c r="D35" s="32" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E35" s="33" t="s">
         <v>145</v>
@@ -14057,7 +14048,7 @@
       <c r="A36" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B36" s="101"/>
+      <c r="B36" s="100"/>
       <c r="C36" s="41"/>
       <c r="D36" s="32" t="s">
         <v>330</v>
@@ -14407,10 +14398,10 @@
       <c r="A37" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B37" s="101"/>
+      <c r="B37" s="100"/>
       <c r="C37" s="44"/>
       <c r="D37" s="32" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E37" s="33" t="s">
         <v>145</v>
@@ -14721,10 +14712,10 @@
       <c r="A38" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B38" s="101"/>
+      <c r="B38" s="100"/>
       <c r="C38" s="44"/>
       <c r="D38" s="32" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E38" s="33" t="s">
         <v>145</v>
@@ -15041,10 +15032,10 @@
       <c r="A39" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B39" s="101"/>
+      <c r="B39" s="100"/>
       <c r="C39" s="44"/>
       <c r="D39" s="32" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E39" s="33" t="s">
         <v>145</v>
@@ -15343,7 +15334,7 @@
         <v>1</v>
       </c>
       <c r="EA39" s="33" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="EB39" s="33" t="s">
         <v>212</v>
@@ -15399,10 +15390,10 @@
       <c r="A40" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B40" s="101"/>
+      <c r="B40" s="100"/>
       <c r="C40" s="44"/>
       <c r="D40" s="32" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E40" s="33" t="s">
         <v>145</v>
@@ -15691,7 +15682,7 @@
         <v>1</v>
       </c>
       <c r="EA40" s="33" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="EB40" s="33" t="s">
         <v>212</v>
@@ -15747,10 +15738,10 @@
       <c r="A41" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B41" s="101"/>
+      <c r="B41" s="100"/>
       <c r="C41" s="44"/>
       <c r="D41" s="32" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E41" s="33" t="s">
         <v>145</v>
@@ -16045,7 +16036,7 @@
         <v>1</v>
       </c>
       <c r="EA41" s="33" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="EB41" s="33" t="s">
         <v>212</v>
@@ -16101,10 +16092,10 @@
       <c r="A42" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B42" s="101"/>
+      <c r="B42" s="100"/>
       <c r="C42" s="41"/>
       <c r="D42" s="32" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E42" s="33" t="s">
         <v>145</v>
@@ -16411,10 +16402,10 @@
       <c r="A43" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B43" s="101"/>
+      <c r="B43" s="100"/>
       <c r="C43" s="47"/>
       <c r="D43" s="48" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E43" s="33" t="s">
         <v>145</v>
@@ -16719,10 +16710,10 @@
       <c r="A44" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="B44" s="102"/>
+      <c r="B44" s="101"/>
       <c r="C44" s="49"/>
       <c r="D44" s="50" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E44" s="51" t="s">
         <v>145</v>
@@ -17073,14 +17064,14 @@
       <c r="A45" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="B45" s="103" t="s">
+      <c r="B45" s="102" t="s">
         <v>356</v>
       </c>
       <c r="C45" s="61" t="s">
         <v>357</v>
       </c>
       <c r="D45" s="62" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E45" s="63" t="s">
         <v>145</v>
@@ -17421,7 +17412,7 @@
       <c r="A46" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="B46" s="104"/>
+      <c r="B46" s="103"/>
       <c r="C46" s="71" t="s">
         <v>361</v>
       </c>
@@ -17711,12 +17702,12 @@
       <c r="A47" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="B47" s="104"/>
+      <c r="B47" s="103"/>
       <c r="C47" s="71" t="s">
         <v>365</v>
       </c>
       <c r="D47" s="72" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E47" s="73" t="s">
         <v>145</v>
@@ -17993,7 +17984,7 @@
         <v>0</v>
       </c>
       <c r="EA47" s="73" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="EB47" s="73" t="s">
         <v>212</v>
@@ -18049,12 +18040,12 @@
       <c r="A48" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="B48" s="104"/>
+      <c r="B48" s="103"/>
       <c r="C48" s="71" t="s">
         <v>368</v>
       </c>
       <c r="D48" s="72" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E48" s="73" t="s">
         <v>145</v>
@@ -18359,7 +18350,7 @@
       <c r="A49" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="B49" s="104"/>
+      <c r="B49" s="103"/>
       <c r="C49" s="71" t="s">
         <v>370</v>
       </c>
@@ -18651,12 +18642,12 @@
       <c r="A50" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="B50" s="104"/>
+      <c r="B50" s="103"/>
       <c r="C50" s="71" t="s">
         <v>376</v>
       </c>
       <c r="D50" s="72" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E50" s="73" t="s">
         <v>145</v>
@@ -18991,7 +18982,7 @@
       <c r="A51" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="B51" s="104"/>
+      <c r="B51" s="103"/>
       <c r="C51" s="71" t="s">
         <v>386</v>
       </c>
@@ -19293,12 +19284,12 @@
       <c r="A52" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="B52" s="104"/>
+      <c r="B52" s="103"/>
       <c r="C52" s="71" t="s">
         <v>390</v>
       </c>
       <c r="D52" s="72" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E52" s="73" t="s">
         <v>145</v>
@@ -19637,7 +19628,7 @@
       <c r="A53" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="B53" s="104"/>
+      <c r="B53" s="103"/>
       <c r="C53" s="71" t="s">
         <v>396</v>
       </c>
@@ -19710,7 +19701,7 @@
       </c>
       <c r="AA53" s="73"/>
       <c r="AB53" s="73" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AC53" s="73" t="s">
         <v>401</v>
@@ -19943,12 +19934,12 @@
       <c r="A54" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="B54" s="104"/>
+      <c r="B54" s="103"/>
       <c r="C54" s="71" t="s">
         <v>403</v>
       </c>
       <c r="D54" s="72" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E54" s="73" t="s">
         <v>145</v>
@@ -20289,7 +20280,7 @@
       <c r="A55" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="B55" s="104"/>
+      <c r="B55" s="103"/>
       <c r="C55" s="71" t="s">
         <v>408</v>
       </c>
@@ -20605,12 +20596,12 @@
       <c r="A56" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="B56" s="104"/>
+      <c r="B56" s="103"/>
       <c r="C56" s="71" t="s">
         <v>413</v>
       </c>
       <c r="D56" s="72" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E56" s="73" t="s">
         <v>145</v>
@@ -20921,12 +20912,12 @@
       <c r="A57" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="B57" s="104"/>
+      <c r="B57" s="103"/>
       <c r="C57" s="71" t="s">
         <v>416</v>
       </c>
       <c r="D57" s="72" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E57" s="73" t="s">
         <v>145</v>
@@ -21235,12 +21226,12 @@
       <c r="A58" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="B58" s="104"/>
+      <c r="B58" s="103"/>
       <c r="C58" s="71" t="s">
         <v>420</v>
       </c>
       <c r="D58" s="72" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E58" s="73" t="s">
         <v>145</v>
@@ -21561,12 +21552,12 @@
       <c r="A59" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="B59" s="104"/>
+      <c r="B59" s="103"/>
       <c r="C59" s="71" t="s">
         <v>424</v>
       </c>
       <c r="D59" s="72" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E59" s="73" t="s">
         <v>145</v>
@@ -21881,12 +21872,12 @@
       <c r="A60" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="B60" s="104"/>
+      <c r="B60" s="103"/>
       <c r="C60" s="71" t="s">
         <v>427</v>
       </c>
       <c r="D60" s="72" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E60" s="73" t="s">
         <v>145</v>
@@ -22203,7 +22194,7 @@
       <c r="A61" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="B61" s="104"/>
+      <c r="B61" s="103"/>
       <c r="C61" s="71" t="s">
         <v>428</v>
       </c>
@@ -22525,9 +22516,9 @@
       <c r="A62" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="B62" s="104"/>
+      <c r="B62" s="103"/>
       <c r="C62" s="71" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D62" s="72" t="s">
         <v>431</v>
@@ -22835,16 +22826,16 @@
       </c>
       <c r="ER62" s="29"/>
     </row>
-    <row r="63" spans="1:148" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:148" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="B63" s="104"/>
+      <c r="B63" s="103"/>
       <c r="C63" s="71" t="s">
         <v>433</v>
       </c>
       <c r="D63" s="72" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E63" s="73" t="s">
         <v>145</v>
@@ -22934,9 +22925,7 @@
       <c r="AH63" s="73" t="s">
         <v>159</v>
       </c>
-      <c r="AI63" s="74" t="s">
-        <v>434</v>
-      </c>
+      <c r="AI63" s="74"/>
       <c r="AJ63" s="74"/>
       <c r="AK63" s="74"/>
       <c r="AL63" s="74"/>
@@ -22977,7 +22966,7 @@
       <c r="BS63" s="74"/>
       <c r="BT63" s="74"/>
       <c r="BU63" s="74" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="BV63" s="77" t="s">
         <v>201</v>
@@ -23092,7 +23081,7 @@
         <v>231</v>
       </c>
       <c r="DJ63" s="74">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="DK63" s="74">
         <v>20</v>
@@ -23141,20 +23130,20 @@
       <c r="EQ63" s="24" t="s">
         <v>220</v>
       </c>
-      <c r="ER63" s="29" t="s">
-        <v>436</v>
+      <c r="ER63" s="30" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="64" spans="1:148" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="22" t="b">
         <v>1</v>
       </c>
-      <c r="B64" s="104"/>
+      <c r="B64" s="103"/>
       <c r="C64" s="71" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D64" s="72" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E64" s="73" t="s">
         <v>145</v>
@@ -23244,9 +23233,7 @@
       <c r="AH64" s="73" t="s">
         <v>159</v>
       </c>
-      <c r="AI64" s="74" t="s">
-        <v>434</v>
-      </c>
+      <c r="AI64" s="74"/>
       <c r="AJ64" s="74"/>
       <c r="AK64" s="74"/>
       <c r="AL64" s="74"/>
@@ -23286,7 +23273,9 @@
       <c r="BR64" s="74"/>
       <c r="BS64" s="74"/>
       <c r="BT64" s="74"/>
-      <c r="BU64" s="74"/>
+      <c r="BU64" s="74" t="s">
+        <v>434</v>
+      </c>
       <c r="BV64" s="77" t="s">
         <v>201</v>
       </c>
@@ -23397,7 +23386,7 @@
         <v>100</v>
       </c>
       <c r="DI64" s="74" t="s">
-        <v>231</v>
+        <v>149</v>
       </c>
       <c r="DJ64" s="74">
         <v>10</v>
@@ -23442,19 +23431,19 @@
         <v>220</v>
       </c>
       <c r="ER64" s="30" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="65" spans="1:146" x14ac:dyDescent="0.2">
-      <c r="A65" s="99" t="s">
-        <v>478</v>
-      </c>
-      <c r="B65" s="104"/>
+      <c r="A65" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="B65" s="103"/>
       <c r="C65" s="90" t="s">
+        <v>474</v>
+      </c>
+      <c r="D65" s="91" t="s">
         <v>475</v>
-      </c>
-      <c r="D65" s="91" t="s">
-        <v>476</v>
       </c>
       <c r="E65" s="92" t="s">
         <v>145</v>
@@ -23545,7 +23534,7 @@
         <v>159</v>
       </c>
       <c r="AI65" s="92" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="AJ65" s="92"/>
       <c r="AK65" s="92"/>

</xml_diff>

<commit_message>
TP#15226 Fix integration tests.
Was sending direct when for indirect shipments
When return clearance, send returnclearance as special service instead of return shipment.
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/US Exp Intl.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/US Exp Intl.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4288" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4290" uniqueCount="478">
   <si>
     <t>SaveLabel</t>
   </si>
@@ -1459,6 +1459,9 @@
   </si>
   <si>
     <t>THIRD PARTY CONSIGNEE</t>
+  </si>
+  <si>
+    <t>RETURNS_CLEARANCE</t>
   </si>
 </sst>
 </file>
@@ -2506,10 +2509,10 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:ER65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DF1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z1" sqref="Z1"/>
-      <selection pane="bottomLeft" activeCell="DJ64" sqref="DJ64"/>
+      <selection pane="bottomLeft" activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2627,7 +2630,9 @@
     <col min="122" max="122" width="33.85546875" style="22" customWidth="1"/>
     <col min="123" max="123" width="34.28515625" style="22" customWidth="1"/>
     <col min="124" max="124" width="23" style="22" customWidth="1"/>
-    <col min="125" max="128" width="9.140625" style="22"/>
+    <col min="125" max="125" width="9.140625" style="22"/>
+    <col min="126" max="126" width="40.7109375" style="22" customWidth="1"/>
+    <col min="127" max="128" width="9.140625" style="22"/>
     <col min="129" max="129" width="22.42578125" style="22" customWidth="1"/>
     <col min="130" max="130" width="18.85546875" style="22" customWidth="1"/>
     <col min="131" max="132" width="21" style="22" customWidth="1"/>
@@ -22925,7 +22930,9 @@
       <c r="AH63" s="73" t="s">
         <v>159</v>
       </c>
-      <c r="AI63" s="74"/>
+      <c r="AI63" s="74" t="s">
+        <v>477</v>
+      </c>
       <c r="AJ63" s="74"/>
       <c r="AK63" s="74"/>
       <c r="AL63" s="74"/>
@@ -23233,7 +23240,9 @@
       <c r="AH64" s="73" t="s">
         <v>159</v>
       </c>
-      <c r="AI64" s="74"/>
+      <c r="AI64" s="74" t="s">
+        <v>477</v>
+      </c>
       <c r="AJ64" s="74"/>
       <c r="AK64" s="74"/>
       <c r="AL64" s="74"/>

</xml_diff>

<commit_message>
TP#20088:  Needed mapping for battery fields for us exp intl and added dangerous_goods to the sheet to get them to show up in the request.
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/US Exp Intl.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/US Exp Intl.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4491" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4493" uniqueCount="499">
   <si>
     <t>FEDEX BUSINESS</t>
   </si>
@@ -1519,6 +1519,9 @@
   </si>
   <si>
     <t xml:space="preserve">SaveLabel </t>
+  </si>
+  <si>
+    <t>RequestedShipment.RequestedPackageLineItems.SpecialServicesRequested(Repetitions)2</t>
   </si>
 </sst>
 </file>
@@ -3600,10 +3603,10 @@
   </sheetPr>
   <dimension ref="A1:ER70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="EC1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="DN1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D18" sqref="D18"/>
-      <selection pane="bottomLeft" activeCell="BZ69" sqref="BZ69"/>
+      <selection pane="bottomLeft" activeCell="DQ66" sqref="DQ66:DQ67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4105,7 +4108,7 @@
         <v>274</v>
       </c>
       <c r="DR1" s="27" t="s">
-        <v>274</v>
+        <v>498</v>
       </c>
       <c r="DS1" s="27" t="s">
         <v>478</v>
@@ -24973,7 +24976,9 @@
       <c r="DP66" s="71" t="s">
         <v>365</v>
       </c>
-      <c r="DQ66" s="71"/>
+      <c r="DQ66" s="2" t="s">
+        <v>204</v>
+      </c>
       <c r="DR66" s="71"/>
       <c r="DS66" s="71"/>
       <c r="DT66" s="71"/>
@@ -25281,7 +25286,9 @@
       <c r="DP67" s="76" t="s">
         <v>365</v>
       </c>
-      <c r="DQ67" s="76"/>
+      <c r="DQ67" s="2" t="s">
+        <v>204</v>
+      </c>
       <c r="DR67" s="76"/>
       <c r="DS67" s="76"/>
       <c r="DT67" s="76"/>

</xml_diff>